<commit_message>
Converting experiment type to run type
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Experiment_Infinium_24_vtest.xlsx
+++ b/backend/fms_core/tests/valid_templates/Experiment_Infinium_24_vtest.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A771FB8-94DA-4F42-9DC7-B697A7E6A7AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1760" windowWidth="25080" windowHeight="12980" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Experiments" sheetId="1" r:id="rId1"/>
-    <sheet name="Samples" sheetId="2" r:id="rId2"/>
-    <sheet name="Work" sheetId="3" r:id="rId3"/>
+    <sheet name="Experiments" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Samples" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Work" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -42,11 +37,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Infinium chip Barcode</t>
+          <t xml:space="preserve">Infinium chip Barcode</t>
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="F10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,11 +51,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>provided with the kit</t>
+          <t xml:space="preserve">provided with the kit</t>
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="K10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -70,11 +65,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>date and time</t>
+          <t xml:space="preserve">date and time</t>
         </r>
       </text>
     </comment>
-    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="L10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,11 +79,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>date and time</t>
+          <t xml:space="preserve">date and time</t>
         </r>
       </text>
     </comment>
-    <comment ref="S10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="S10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -98,11 +93,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>until 4 barcodes per 96 well plate for 24 Sentrix format chip</t>
+          <t xml:space="preserve">until 4 barcodes per 96 well plate for 24 Sentrix format chip</t>
         </r>
       </text>
     </comment>
-    <comment ref="W10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="W10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -112,11 +107,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>date and time</t>
+          <t xml:space="preserve">date and time</t>
         </r>
       </text>
     </comment>
-    <comment ref="X10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="X10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -126,11 +121,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>date and time</t>
+          <t xml:space="preserve">date and time</t>
         </r>
       </text>
     </comment>
-    <comment ref="AM10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="AM10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,11 +135,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>This field is present only for lab validation. It will not be stored. It should match Experiment Container Barcode.</t>
+          <t xml:space="preserve">This field is present only for lab validation. It will not be stored. It should match Experiment Container Barcode.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AN10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="AN10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +149,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>can handle 4 chip max</t>
+          <t xml:space="preserve">can handle 4 chip max</t>
         </r>
       </text>
     </comment>
@@ -165,341 +160,343 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
   <si>
-    <t>Experiment Submission Template</t>
-  </si>
-  <si>
-    <t>Experiment Type</t>
-  </si>
-  <si>
-    <t>Template Version</t>
-  </si>
-  <si>
-    <t>Fill the Experiments page with the information common to all samples in each experiment, then detail information specific to each sample on the Samples page.</t>
-  </si>
-  <si>
-    <t>If a sample appears in more than one experiment, enter multiple entries with the information pertaining to each experiment with the appropriate experiment ID.</t>
-  </si>
-  <si>
-    <t>Experiment</t>
-  </si>
-  <si>
-    <t>Amplification</t>
-  </si>
-  <si>
-    <t>Fragmentation</t>
-  </si>
-  <si>
-    <t>Precipitation</t>
-  </si>
-  <si>
-    <t>Hybridization</t>
-  </si>
-  <si>
-    <t>Wash beadchip</t>
-  </si>
-  <si>
-    <t>Extend and Stain</t>
-  </si>
-  <si>
-    <t>Image (scan)</t>
-  </si>
-  <si>
-    <t>Experiment ID</t>
-  </si>
-  <si>
-    <t>Experiment Container Barcode</t>
-  </si>
-  <si>
-    <t>Experiment Container Kind</t>
-  </si>
-  <si>
-    <t>Instrument Name</t>
-  </si>
-  <si>
-    <t>Experiment Start Date</t>
-  </si>
-  <si>
-    <t>MSA3 Plate Barcode</t>
-  </si>
-  <si>
-    <t>0.1N NaOH formulation date</t>
-  </si>
-  <si>
-    <t>Reagent MA1 Barcode</t>
-  </si>
-  <si>
-    <t>Reagent MA2 Barcode</t>
-  </si>
-  <si>
-    <t>Reagent MSM Barcode</t>
-  </si>
-  <si>
-    <t>Incubation time In Amplification</t>
-  </si>
-  <si>
-    <t>Incubation time Out Amplification</t>
-  </si>
-  <si>
-    <t>Comment Amplification</t>
-  </si>
-  <si>
-    <t>Reagent FMS Barcode</t>
-  </si>
-  <si>
-    <t>Comment Fragmentation</t>
-  </si>
-  <si>
-    <t>Reagent PM1 Barcode</t>
-  </si>
-  <si>
-    <t>Reagent RA1 Barcode Precipitation</t>
-  </si>
-  <si>
-    <t>Comment Precipitation</t>
-  </si>
-  <si>
-    <t>Hybridization Chip Barcodes</t>
-  </si>
-  <si>
-    <t>Hybridization Chamber Barcode</t>
-  </si>
-  <si>
-    <t>Reagent PB2 Barcode</t>
-  </si>
-  <si>
-    <t>Reagent XC4 Barcode Hybridization</t>
-  </si>
-  <si>
-    <t>Incubation time In Hybridization</t>
-  </si>
-  <si>
-    <t>Incubation time Out Hybridization</t>
-  </si>
-  <si>
-    <t>Comment Hybridization</t>
-  </si>
-  <si>
-    <t>Reagent PB1 Barcode Wash</t>
-  </si>
-  <si>
-    <t>Comment Wash</t>
-  </si>
-  <si>
-    <t>95% form/EDTA</t>
-  </si>
-  <si>
-    <t>Reagent ATM Barcode</t>
-  </si>
-  <si>
-    <t>Reagent EML Barcode</t>
-  </si>
-  <si>
-    <t>Reagent LX1 Barcode</t>
-  </si>
-  <si>
-    <t>Reagent LX2 Barcode</t>
-  </si>
-  <si>
-    <t>Reagent PB1 Barcode Stain</t>
-  </si>
-  <si>
-    <t>Reagent RA1 Barcode Stain</t>
-  </si>
-  <si>
-    <t>Reagent SML Barcode</t>
-  </si>
-  <si>
-    <t>Reagent XC3 Barcode</t>
-  </si>
-  <si>
-    <t>Reagent XC4 Barcode Stain</t>
-  </si>
-  <si>
-    <t>Comment Stain</t>
-  </si>
-  <si>
-    <t>SentrixBarcode_A</t>
-  </si>
-  <si>
-    <t>Scan Chip Rack Barcode</t>
-  </si>
-  <si>
-    <t>Comment Scan</t>
-  </si>
-  <si>
-    <t>Sample Preparation</t>
-  </si>
-  <si>
-    <t>Source Container Barcode</t>
-  </si>
-  <si>
-    <t>Source Container Position</t>
-  </si>
-  <si>
-    <t>Source Sample Volume Used</t>
-  </si>
-  <si>
-    <t>Experiment Container Position</t>
-  </si>
-  <si>
-    <t>Fragment</t>
-  </si>
-  <si>
-    <t>Precipitate and Resuspend</t>
-  </si>
-  <si>
-    <t>Hybridize</t>
-  </si>
-  <si>
-    <t>Wash BeadChip</t>
-  </si>
-  <si>
-    <t>Image (Scan)</t>
-  </si>
-  <si>
-    <t>MSA3 Plate Barcode (provides with the kit)</t>
-  </si>
-  <si>
-    <t>Chip Barcodes (until 4 barcodes per 96 well plate for 24 Sentrix format chip)</t>
-  </si>
-  <si>
-    <t>Reagent PB1 Barcode</t>
-  </si>
-  <si>
-    <t>Chip Barcode (until 4 barcodes per 96 well plate for 24 Sentrix format chip)</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Reagent RA1 Barcode</t>
-  </si>
-  <si>
-    <t>Chip Rack Barcode (can handle 4 chip max)</t>
-  </si>
-  <si>
-    <t>Reagent XC4 Barcode</t>
-  </si>
-  <si>
-    <t>Incubation time In (date and time)</t>
-  </si>
-  <si>
-    <t>Incubation time Out (date and time)</t>
-  </si>
-  <si>
-    <t>TestExp</t>
-  </si>
-  <si>
-    <t>infinium gs 24 beadchip</t>
-  </si>
-  <si>
-    <t>iScan_1</t>
-  </si>
-  <si>
-    <t>PlateBarcode</t>
-  </si>
-  <si>
-    <t>ReagentAmpBarcode</t>
-  </si>
-  <si>
-    <t>ReagentMA2BarcodeHere</t>
-  </si>
-  <si>
-    <t>MSMBarcode</t>
-  </si>
-  <si>
-    <t>FragFMSBarcode</t>
-  </si>
-  <si>
-    <t>short comment</t>
-  </si>
-  <si>
-    <t>Pm1Barcode</t>
-  </si>
-  <si>
-    <t>Ra1PrecipBarcode</t>
-  </si>
-  <si>
-    <t>HybrBarcodeValue</t>
-  </si>
-  <si>
-    <t>HCBarcode</t>
-  </si>
-  <si>
-    <t>PB2Barcode</t>
-  </si>
-  <si>
-    <t>XC4HyBarcode</t>
-  </si>
-  <si>
-    <t>my comment</t>
-  </si>
-  <si>
-    <t>washbeadchipbarcode</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>atmbarcodehere</t>
-  </si>
-  <si>
-    <t>testbarcode</t>
-  </si>
-  <si>
-    <t>lx1barcode</t>
-  </si>
-  <si>
-    <t>lx2barcode</t>
-  </si>
-  <si>
-    <t>pb1stain</t>
-  </si>
-  <si>
-    <t>ra1stain</t>
-  </si>
-  <si>
-    <t>smltest</t>
-  </si>
-  <si>
-    <t>xc3value</t>
-  </si>
-  <si>
-    <t>xc4stain</t>
-  </si>
-  <si>
-    <t>sentrixA</t>
-  </si>
-  <si>
-    <t>lastbarcode</t>
-  </si>
-  <si>
-    <t>bla bla bla</t>
-  </si>
-  <si>
-    <t>Infinium Global Screening Array-24</t>
-  </si>
-  <si>
-    <t>A01</t>
-  </si>
-  <si>
-    <t>EQ00539851</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>Test</t>
+    <t xml:space="preserve">Experiment Submission Template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infinium Global Screening Array-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Template Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill the Experiments page with the information common to all samples in each experiment, then detail information specific to each sample on the Samples page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If a sample appears in more than one experiment, enter multiple entries with the information pertaining to each experiment with the appropriate experiment ID.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amplification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fragmentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybridization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wash beadchip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extend and Stain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image (scan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment Container Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment Container Kind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instrument Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment Start Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSA3 Plate Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1N NaOH formulation date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent MA1 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent MA2 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent MSM Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incubation time In Amplification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incubation time Out Amplification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment Amplification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent FMS Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment Fragmentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent PM1 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent RA1 Barcode Precipitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment Precipitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybridization Chip Barcodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybridization Chamber Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent PB2 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent XC4 Barcode Hybridization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incubation time In Hybridization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incubation time Out Hybridization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment Hybridization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent PB1 Barcode Wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment Wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95% form/EDTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent ATM Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent EML Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent LX1 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent LX2 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent PB1 Barcode Stain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent RA1 Barcode Stain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent SML Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent XC3 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent XC4 Barcode Stain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment Stain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SentrixBarcode_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scan Chip Rack Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment Scan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestExp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infinium gs 24 beadchip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iScan_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PlateBarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReagentAmpBarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReagentMA2BarcodeHere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSMBarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FragFMSBarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">short comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pm1Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ra1PrecipBarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HybrBarcodeValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCBarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB2Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XC4HyBarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">washbeadchipbarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atmbarcodehere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testbarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lx1barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lx2barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pb1stain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ra1stain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smltest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xc3value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xc4stain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sentrixA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastbarcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bla bla bla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Preparation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source Container Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source Container Coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source Sample Volume Used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment Container Coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EQ00539851</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fragment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitate and Resuspend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybridize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wash BeadChip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image (Scan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSA3 Plate Barcode (provides with the kit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip Barcodes (until 4 barcodes per 96 well plate for 24 Sentrix format chip)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent PB1 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip Barcode (until 4 barcodes per 96 well plate for 24 Sentrix format chip)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent RA1 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip Rack Barcode (can handle 4 chip max)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reagent XC4 Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incubation time In (date and time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incubation time Out (date and time)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -508,7 +505,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -599,130 +611,213 @@
     </fill>
   </fills>
   <borders count="5">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
+      <right style="dashed"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="34">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -772,7 +867,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF999999"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -781,430 +876,122 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F497D"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AMI106"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="2" width="48.5" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
-    <col min="7" max="7" width="27.5" customWidth="1"/>
-    <col min="8" max="9" width="21.1640625" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" customWidth="1"/>
-    <col min="11" max="11" width="26.6640625" customWidth="1"/>
-    <col min="12" max="12" width="27.83203125" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" customWidth="1"/>
-    <col min="14" max="14" width="21" customWidth="1"/>
-    <col min="15" max="15" width="20.83203125" customWidth="1"/>
-    <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="28.83203125" customWidth="1"/>
-    <col min="18" max="18" width="19.1640625" customWidth="1"/>
-    <col min="19" max="19" width="23.1640625" customWidth="1"/>
-    <col min="20" max="20" width="26.1640625" customWidth="1"/>
-    <col min="21" max="21" width="20.5" customWidth="1"/>
-    <col min="22" max="22" width="32" customWidth="1"/>
-    <col min="23" max="23" width="26.6640625" customWidth="1"/>
-    <col min="24" max="24" width="35" customWidth="1"/>
-    <col min="25" max="25" width="19.6640625" customWidth="1"/>
-    <col min="26" max="26" width="22.83203125" customWidth="1"/>
-    <col min="27" max="27" width="13.6640625" customWidth="1"/>
-    <col min="28" max="28" width="19.1640625" customWidth="1"/>
-    <col min="29" max="29" width="21.1640625" customWidth="1"/>
-    <col min="30" max="30" width="20.83203125" customWidth="1"/>
-    <col min="31" max="32" width="20.1640625" customWidth="1"/>
-    <col min="33" max="33" width="23.5" customWidth="1"/>
-    <col min="34" max="34" width="22.83203125" customWidth="1"/>
-    <col min="35" max="35" width="18.5" customWidth="1"/>
-    <col min="36" max="36" width="18.1640625" customWidth="1"/>
-    <col min="37" max="37" width="22.6640625" customWidth="1"/>
-    <col min="38" max="38" width="13.5" customWidth="1"/>
-    <col min="39" max="40" width="25.5" customWidth="1"/>
-    <col min="41" max="41" width="15.1640625" customWidth="1"/>
-    <col min="1019" max="1023" width="9.1640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="26.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="18.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="18.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="15.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1019" style="0" width="9.17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:1023" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="6" spans="1:1023" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1023" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10"/>
     </row>
-    <row r="9" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -1214,16 +1001,16 @@
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O9" s="15"/>
       <c r="P9" s="16" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
       <c r="S9" s="17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="T9" s="17"/>
       <c r="U9" s="17"/>
@@ -1232,11 +1019,11 @@
       <c r="X9" s="17"/>
       <c r="Y9" s="17"/>
       <c r="Z9" s="18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA9" s="18"/>
       <c r="AB9" s="19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AC9" s="19"/>
       <c r="AD9" s="19"/>
@@ -1249,134 +1036,134 @@
       <c r="AK9" s="19"/>
       <c r="AL9" s="19"/>
       <c r="AM9" s="20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AN9" s="20"/>
       <c r="AO9" s="20"/>
     </row>
-    <row r="10" spans="1:1023" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R10" s="21" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S10" s="21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="T10" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U10" s="21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="V10" s="21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="W10" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="X10" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Y10" s="21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Z10" s="21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AA10" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AB10" s="21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AC10" s="21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AD10" s="21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AE10" s="21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AF10" s="21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AG10" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AH10" s="21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AI10" s="21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AJ10" s="21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AK10" s="21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AL10" s="21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AM10" s="21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AN10" s="21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AO10" s="21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AME10" s="21"/>
       <c r="AMF10" s="21"/>
@@ -1384,125 +1171,125 @@
       <c r="AMH10" s="21"/>
       <c r="AMI10" s="21"/>
     </row>
-    <row r="11" spans="1:1023" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="25" t="n">
+        <v>44198</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>44289</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="27" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="L11" s="27" t="n">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="S11" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="W11" s="27" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="X11" s="27" t="n">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z11" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB11" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="AC11" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D11" t="s">
+      <c r="AD11" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="30">
-        <v>44198</v>
-      </c>
-      <c r="F11" s="31" t="s">
+      <c r="AE11" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="1">
-        <v>44289</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="AF11" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="I11" t="s">
+      <c r="AG11" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="J11" t="s">
+      <c r="AH11" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="32">
-        <v>0.125</v>
-      </c>
-      <c r="L11" s="32">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="N11" s="29" t="s">
+      <c r="AI11" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="O11" t="s">
+      <c r="AJ11" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="P11" s="29" t="s">
+      <c r="AK11" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="AM11" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="S11" s="29" t="s">
+      <c r="AN11" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="T11" t="s">
+      <c r="AO11" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="U11" t="s">
-        <v>87</v>
-      </c>
-      <c r="V11" t="s">
-        <v>88</v>
-      </c>
-      <c r="W11" s="32">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="X11" s="32">
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z11" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB11" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>93</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>95</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>98</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>99</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>100</v>
-      </c>
-      <c r="AM11" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO11" s="33" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1023" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="24"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1540,12 +1327,12 @@
       <c r="AN12" s="10"/>
       <c r="AO12" s="10"/>
     </row>
-    <row r="13" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="24"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -1583,12 +1370,12 @@
       <c r="AN13" s="10"/>
       <c r="AO13" s="10"/>
     </row>
-    <row r="14" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="24"/>
+      <c r="E14" s="29"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1626,12 +1413,12 @@
       <c r="AN14" s="10"/>
       <c r="AO14" s="10"/>
     </row>
-    <row r="15" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="24"/>
+      <c r="E15" s="29"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -1669,12 +1456,12 @@
       <c r="AN15" s="10"/>
       <c r="AO15" s="10"/>
     </row>
-    <row r="16" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="24"/>
+      <c r="E16" s="29"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
@@ -1712,12 +1499,12 @@
       <c r="AN16" s="10"/>
       <c r="AO16" s="10"/>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="24"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1755,12 +1542,12 @@
       <c r="AN17" s="10"/>
       <c r="AO17" s="10"/>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="24"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
@@ -1798,12 +1585,12 @@
       <c r="AN18" s="10"/>
       <c r="AO18" s="10"/>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="24"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -1841,12 +1628,12 @@
       <c r="AN19" s="10"/>
       <c r="AO19" s="10"/>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="24"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
@@ -1884,12 +1671,12 @@
       <c r="AN20" s="10"/>
       <c r="AO20" s="10"/>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="24"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
@@ -1927,12 +1714,12 @@
       <c r="AN21" s="10"/>
       <c r="AO21" s="10"/>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="24"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -1970,12 +1757,12 @@
       <c r="AN22" s="10"/>
       <c r="AO22" s="10"/>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="24"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -2013,12 +1800,12 @@
       <c r="AN23" s="10"/>
       <c r="AO23" s="10"/>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="24"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
@@ -2056,12 +1843,12 @@
       <c r="AN24" s="10"/>
       <c r="AO24" s="10"/>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="24"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -2099,12 +1886,12 @@
       <c r="AN25" s="10"/>
       <c r="AO25" s="10"/>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="24"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -2142,12 +1929,12 @@
       <c r="AN26" s="10"/>
       <c r="AO26" s="10"/>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="24"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -2185,12 +1972,12 @@
       <c r="AN27" s="10"/>
       <c r="AO27" s="10"/>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
-      <c r="E28" s="24"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -2228,12 +2015,12 @@
       <c r="AN28" s="10"/>
       <c r="AO28" s="10"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
-      <c r="E29" s="24"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -2271,12 +2058,12 @@
       <c r="AN29" s="10"/>
       <c r="AO29" s="10"/>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
-      <c r="E30" s="24"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -2314,12 +2101,12 @@
       <c r="AN30" s="10"/>
       <c r="AO30" s="10"/>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
-      <c r="E31" s="24"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
@@ -2357,12 +2144,12 @@
       <c r="AN31" s="10"/>
       <c r="AO31" s="10"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
-      <c r="E32" s="24"/>
+      <c r="E32" s="29"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -2400,12 +2187,12 @@
       <c r="AN32" s="10"/>
       <c r="AO32" s="10"/>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
-      <c r="E33" s="24"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
@@ -2443,12 +2230,12 @@
       <c r="AN33" s="10"/>
       <c r="AO33" s="10"/>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
-      <c r="E34" s="24"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -2486,12 +2273,12 @@
       <c r="AN34" s="10"/>
       <c r="AO34" s="10"/>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
-      <c r="E35" s="24"/>
+      <c r="E35" s="29"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -2529,12 +2316,12 @@
       <c r="AN35" s="10"/>
       <c r="AO35" s="10"/>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
-      <c r="E36" s="24"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
@@ -2572,12 +2359,12 @@
       <c r="AN36" s="10"/>
       <c r="AO36" s="10"/>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
-      <c r="E37" s="24"/>
+      <c r="E37" s="29"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
@@ -2615,12 +2402,12 @@
       <c r="AN37" s="10"/>
       <c r="AO37" s="10"/>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
-      <c r="E38" s="24"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
@@ -2658,12 +2445,12 @@
       <c r="AN38" s="10"/>
       <c r="AO38" s="10"/>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
-      <c r="E39" s="24"/>
+      <c r="E39" s="29"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
@@ -2701,12 +2488,12 @@
       <c r="AN39" s="10"/>
       <c r="AO39" s="10"/>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
-      <c r="E40" s="24"/>
+      <c r="E40" s="29"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -2744,12 +2531,12 @@
       <c r="AN40" s="10"/>
       <c r="AO40" s="10"/>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
-      <c r="E41" s="24"/>
+      <c r="E41" s="29"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
@@ -2787,12 +2574,12 @@
       <c r="AN41" s="10"/>
       <c r="AO41" s="10"/>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
-      <c r="E42" s="24"/>
+      <c r="E42" s="29"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -2830,12 +2617,12 @@
       <c r="AN42" s="10"/>
       <c r="AO42" s="10"/>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
-      <c r="E43" s="24"/>
+      <c r="E43" s="29"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
@@ -2873,12 +2660,12 @@
       <c r="AN43" s="10"/>
       <c r="AO43" s="10"/>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
-      <c r="E44" s="24"/>
+      <c r="E44" s="29"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
@@ -2916,12 +2703,12 @@
       <c r="AN44" s="10"/>
       <c r="AO44" s="10"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
-      <c r="E45" s="24"/>
+      <c r="E45" s="29"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
@@ -2959,12 +2746,12 @@
       <c r="AN45" s="10"/>
       <c r="AO45" s="10"/>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
-      <c r="E46" s="24"/>
+      <c r="E46" s="29"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
@@ -3002,12 +2789,12 @@
       <c r="AN46" s="10"/>
       <c r="AO46" s="10"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
-      <c r="E47" s="24"/>
+      <c r="E47" s="29"/>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
@@ -3045,12 +2832,12 @@
       <c r="AN47" s="10"/>
       <c r="AO47" s="10"/>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
-      <c r="E48" s="24"/>
+      <c r="E48" s="29"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
@@ -3088,12 +2875,12 @@
       <c r="AN48" s="10"/>
       <c r="AO48" s="10"/>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
-      <c r="E49" s="24"/>
+      <c r="E49" s="29"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
@@ -3131,12 +2918,12 @@
       <c r="AN49" s="10"/>
       <c r="AO49" s="10"/>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
-      <c r="E50" s="24"/>
+      <c r="E50" s="29"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
@@ -3174,12 +2961,12 @@
       <c r="AN50" s="10"/>
       <c r="AO50" s="10"/>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
-      <c r="E51" s="24"/>
+      <c r="E51" s="29"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
@@ -3217,12 +3004,12 @@
       <c r="AN51" s="10"/>
       <c r="AO51" s="10"/>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="24"/>
+      <c r="E52" s="29"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
@@ -3260,12 +3047,12 @@
       <c r="AN52" s="10"/>
       <c r="AO52" s="10"/>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10"/>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
-      <c r="E53" s="24"/>
+      <c r="E53" s="29"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
@@ -3303,12 +3090,12 @@
       <c r="AN53" s="10"/>
       <c r="AO53" s="10"/>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
-      <c r="E54" s="24"/>
+      <c r="E54" s="29"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
@@ -3346,12 +3133,12 @@
       <c r="AN54" s="10"/>
       <c r="AO54" s="10"/>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
-      <c r="E55" s="24"/>
+      <c r="E55" s="29"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
@@ -3389,12 +3176,12 @@
       <c r="AN55" s="10"/>
       <c r="AO55" s="10"/>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
-      <c r="E56" s="24"/>
+      <c r="E56" s="29"/>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
@@ -3432,12 +3219,12 @@
       <c r="AN56" s="10"/>
       <c r="AO56" s="10"/>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
-      <c r="E57" s="24"/>
+      <c r="E57" s="29"/>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
@@ -3475,12 +3262,12 @@
       <c r="AN57" s="10"/>
       <c r="AO57" s="10"/>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
-      <c r="E58" s="24"/>
+      <c r="E58" s="29"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
@@ -3518,12 +3305,12 @@
       <c r="AN58" s="10"/>
       <c r="AO58" s="10"/>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
-      <c r="E59" s="24"/>
+      <c r="E59" s="29"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
       <c r="H59" s="10"/>
@@ -3561,12 +3348,12 @@
       <c r="AN59" s="10"/>
       <c r="AO59" s="10"/>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
-      <c r="E60" s="24"/>
+      <c r="E60" s="29"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
@@ -3604,12 +3391,12 @@
       <c r="AN60" s="10"/>
       <c r="AO60" s="10"/>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
-      <c r="E61" s="24"/>
+      <c r="E61" s="29"/>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
@@ -3647,12 +3434,12 @@
       <c r="AN61" s="10"/>
       <c r="AO61" s="10"/>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
-      <c r="E62" s="24"/>
+      <c r="E62" s="29"/>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
@@ -3690,12 +3477,12 @@
       <c r="AN62" s="10"/>
       <c r="AO62" s="10"/>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
-      <c r="E63" s="24"/>
+      <c r="E63" s="29"/>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
@@ -3733,12 +3520,12 @@
       <c r="AN63" s="10"/>
       <c r="AO63" s="10"/>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
-      <c r="E64" s="24"/>
+      <c r="E64" s="29"/>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
@@ -3776,12 +3563,12 @@
       <c r="AN64" s="10"/>
       <c r="AO64" s="10"/>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
-      <c r="E65" s="24"/>
+      <c r="E65" s="29"/>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
       <c r="H65" s="10"/>
@@ -3819,12 +3606,12 @@
       <c r="AN65" s="10"/>
       <c r="AO65" s="10"/>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
-      <c r="E66" s="24"/>
+      <c r="E66" s="29"/>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
@@ -3862,12 +3649,12 @@
       <c r="AN66" s="10"/>
       <c r="AO66" s="10"/>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
-      <c r="E67" s="24"/>
+      <c r="E67" s="29"/>
       <c r="F67" s="10"/>
       <c r="G67" s="10"/>
       <c r="H67" s="10"/>
@@ -3905,12 +3692,12 @@
       <c r="AN67" s="10"/>
       <c r="AO67" s="10"/>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
-      <c r="E68" s="24"/>
+      <c r="E68" s="29"/>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
       <c r="H68" s="10"/>
@@ -3948,12 +3735,12 @@
       <c r="AN68" s="10"/>
       <c r="AO68" s="10"/>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
-      <c r="E69" s="24"/>
+      <c r="E69" s="29"/>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
@@ -3991,12 +3778,12 @@
       <c r="AN69" s="10"/>
       <c r="AO69" s="10"/>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
-      <c r="E70" s="24"/>
+      <c r="E70" s="29"/>
       <c r="F70" s="10"/>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
@@ -4034,12 +3821,12 @@
       <c r="AN70" s="10"/>
       <c r="AO70" s="10"/>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
-      <c r="E71" s="24"/>
+      <c r="E71" s="29"/>
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
@@ -4077,12 +3864,12 @@
       <c r="AN71" s="10"/>
       <c r="AO71" s="10"/>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="10"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
-      <c r="E72" s="24"/>
+      <c r="E72" s="29"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
@@ -4120,12 +3907,12 @@
       <c r="AN72" s="10"/>
       <c r="AO72" s="10"/>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="10"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
-      <c r="E73" s="24"/>
+      <c r="E73" s="29"/>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
@@ -4163,12 +3950,12 @@
       <c r="AN73" s="10"/>
       <c r="AO73" s="10"/>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
-      <c r="E74" s="24"/>
+      <c r="E74" s="29"/>
       <c r="F74" s="10"/>
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
@@ -4206,12 +3993,12 @@
       <c r="AN74" s="10"/>
       <c r="AO74" s="10"/>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
-      <c r="E75" s="24"/>
+      <c r="E75" s="29"/>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
@@ -4249,12 +4036,12 @@
       <c r="AN75" s="10"/>
       <c r="AO75" s="10"/>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
-      <c r="E76" s="24"/>
+      <c r="E76" s="29"/>
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
       <c r="H76" s="10"/>
@@ -4292,12 +4079,12 @@
       <c r="AN76" s="10"/>
       <c r="AO76" s="10"/>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="10"/>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
-      <c r="E77" s="24"/>
+      <c r="E77" s="29"/>
       <c r="F77" s="10"/>
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>
@@ -4335,12 +4122,12 @@
       <c r="AN77" s="10"/>
       <c r="AO77" s="10"/>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="10"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
-      <c r="E78" s="24"/>
+      <c r="E78" s="29"/>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
       <c r="H78" s="10"/>
@@ -4378,12 +4165,12 @@
       <c r="AN78" s="10"/>
       <c r="AO78" s="10"/>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
-      <c r="E79" s="24"/>
+      <c r="E79" s="29"/>
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
       <c r="H79" s="10"/>
@@ -4421,12 +4208,12 @@
       <c r="AN79" s="10"/>
       <c r="AO79" s="10"/>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="10"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
-      <c r="E80" s="24"/>
+      <c r="E80" s="29"/>
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
       <c r="H80" s="10"/>
@@ -4464,12 +4251,12 @@
       <c r="AN80" s="10"/>
       <c r="AO80" s="10"/>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="10"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10"/>
-      <c r="E81" s="24"/>
+      <c r="E81" s="29"/>
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
@@ -4507,12 +4294,12 @@
       <c r="AN81" s="10"/>
       <c r="AO81" s="10"/>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10"/>
-      <c r="E82" s="24"/>
+      <c r="E82" s="29"/>
       <c r="F82" s="10"/>
       <c r="G82" s="10"/>
       <c r="H82" s="10"/>
@@ -4550,12 +4337,12 @@
       <c r="AN82" s="10"/>
       <c r="AO82" s="10"/>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="10"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
       <c r="D83" s="10"/>
-      <c r="E83" s="24"/>
+      <c r="E83" s="29"/>
       <c r="F83" s="10"/>
       <c r="G83" s="10"/>
       <c r="H83" s="10"/>
@@ -4593,12 +4380,12 @@
       <c r="AN83" s="10"/>
       <c r="AO83" s="10"/>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
-      <c r="E84" s="24"/>
+      <c r="E84" s="29"/>
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
       <c r="H84" s="10"/>
@@ -4636,12 +4423,12 @@
       <c r="AN84" s="10"/>
       <c r="AO84" s="10"/>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
-      <c r="E85" s="24"/>
+      <c r="E85" s="29"/>
       <c r="F85" s="10"/>
       <c r="G85" s="10"/>
       <c r="H85" s="10"/>
@@ -4679,12 +4466,12 @@
       <c r="AN85" s="10"/>
       <c r="AO85" s="10"/>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
       <c r="D86" s="10"/>
-      <c r="E86" s="24"/>
+      <c r="E86" s="29"/>
       <c r="F86" s="10"/>
       <c r="G86" s="10"/>
       <c r="H86" s="10"/>
@@ -4722,12 +4509,12 @@
       <c r="AN86" s="10"/>
       <c r="AO86" s="10"/>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
       <c r="D87" s="10"/>
-      <c r="E87" s="24"/>
+      <c r="E87" s="29"/>
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
       <c r="H87" s="10"/>
@@ -4765,12 +4552,12 @@
       <c r="AN87" s="10"/>
       <c r="AO87" s="10"/>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
       <c r="D88" s="10"/>
-      <c r="E88" s="24"/>
+      <c r="E88" s="29"/>
       <c r="F88" s="10"/>
       <c r="G88" s="10"/>
       <c r="H88" s="10"/>
@@ -4808,12 +4595,12 @@
       <c r="AN88" s="10"/>
       <c r="AO88" s="10"/>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
       <c r="D89" s="10"/>
-      <c r="E89" s="24"/>
+      <c r="E89" s="29"/>
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
       <c r="H89" s="10"/>
@@ -4851,12 +4638,12 @@
       <c r="AN89" s="10"/>
       <c r="AO89" s="10"/>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
       <c r="D90" s="10"/>
-      <c r="E90" s="24"/>
+      <c r="E90" s="29"/>
       <c r="F90" s="10"/>
       <c r="G90" s="10"/>
       <c r="H90" s="10"/>
@@ -4894,12 +4681,12 @@
       <c r="AN90" s="10"/>
       <c r="AO90" s="10"/>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
       <c r="D91" s="10"/>
-      <c r="E91" s="24"/>
+      <c r="E91" s="29"/>
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
       <c r="H91" s="10"/>
@@ -4937,12 +4724,12 @@
       <c r="AN91" s="10"/>
       <c r="AO91" s="10"/>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
       <c r="D92" s="10"/>
-      <c r="E92" s="24"/>
+      <c r="E92" s="29"/>
       <c r="F92" s="10"/>
       <c r="G92" s="10"/>
       <c r="H92" s="10"/>
@@ -4980,12 +4767,12 @@
       <c r="AN92" s="10"/>
       <c r="AO92" s="10"/>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
       <c r="D93" s="10"/>
-      <c r="E93" s="24"/>
+      <c r="E93" s="29"/>
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
       <c r="H93" s="10"/>
@@ -5023,12 +4810,12 @@
       <c r="AN93" s="10"/>
       <c r="AO93" s="10"/>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
-      <c r="E94" s="24"/>
+      <c r="E94" s="29"/>
       <c r="F94" s="10"/>
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
@@ -5066,12 +4853,12 @@
       <c r="AN94" s="10"/>
       <c r="AO94" s="10"/>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10"/>
-      <c r="E95" s="24"/>
+      <c r="E95" s="29"/>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
@@ -5109,310 +4896,604 @@
       <c r="AN95" s="10"/>
       <c r="AO95" s="10"/>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="10"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="10"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="10"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="10"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="10"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="10"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="10"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="10"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="10"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="10"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMI19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMH100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="982" max="1023" width="9.1640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="982" style="0" width="9.17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>54</v>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30" t="s">
+        <v>87</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:1023" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="26" t="s">
+    <row r="4" s="31" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="AMF4" s="32"/>
+      <c r="AMG4" s="32"/>
+      <c r="AMH4" s="32"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="AMF4" s="27"/>
-      <c r="AMG4" s="27"/>
-      <c r="AMH4" s="27"/>
-      <c r="AMI4"/>
-    </row>
-    <row r="5" spans="1:1023" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="E5" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10"/>
       <c r="C19" s="8"/>
     </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="10"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="10"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="10"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="10"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="10"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="10"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="10"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="10"/>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="10"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="10"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="10"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="10"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="10"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="10"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="10"/>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="10"/>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="10"/>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="10"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="10"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="10"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="10"/>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="10"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="10"/>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="10"/>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="10"/>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="10"/>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="10"/>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="10"/>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="10"/>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="10"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="10"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="10"/>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="10"/>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="10"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="10"/>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="10"/>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="10"/>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="10"/>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="10"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="10"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="10"/>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="10"/>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="10"/>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="10"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="10"/>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="10"/>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="10"/>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="10"/>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="10"/>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="10"/>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="10"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
-          <x14:formula1>
-            <xm:f>Experiments!$A$11:$A$110</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>A5:A100</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
+      <formula1>Experiments!$A$11:$A$110</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-    <col min="4" max="4" width="71.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="70.33203125" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="71.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="70.34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="G2" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="B3" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="G3" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C4" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F12" t="s">
-        <v>68</v>
+      <c r="G4" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>